<commit_message>
Drag Coefficient have been separated in the control data for the super and substructures
</commit_message>
<xml_diff>
--- a/Spread sheet/Wind Load Generator.xlsx
+++ b/Spread sheet/Wind Load Generator.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wind_load_generator\Spread sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB7EBF96-8561-47B2-A30D-DE888E7BF382}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE8D0E5B-5971-4D85-B550-1469A1A923FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Wind Load" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
   <si>
     <t>Load Case</t>
   </si>
@@ -81,6 +81,41 @@
   </si>
   <si>
     <t>Wind Speed</t>
+  </si>
+  <si>
+    <t>Wind Pressures</t>
+  </si>
+  <si>
+    <t>Gust factor</t>
+  </si>
+  <si>
+    <t>Drag Coefficient</t>
+  </si>
+  <si>
+    <t>Skew Coefficients</t>
+  </si>
+  <si>
+    <t>Skew Angle 
+(degree)</t>
+  </si>
+  <si>
+    <t>Transverse Skew Coefficient</t>
+  </si>
+  <si>
+    <t>Longitudinal Skew 
+Coefficient</t>
+  </si>
+  <si>
+    <t>Width for loading along Transverse</t>
+  </si>
+  <si>
+    <t>Width for loading along Longitudinal</t>
+  </si>
+  <si>
+    <t>Transverse Force Component</t>
+  </si>
+  <si>
+    <t>Longitudinal Force Component</t>
   </si>
 </sst>
 </file>
@@ -91,7 +126,7 @@
     <numFmt numFmtId="164" formatCode="#\ &quot;mph&quot;"/>
     <numFmt numFmtId="165" formatCode="#\ &quot;ft&quot;"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -99,16 +134,45 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -116,19 +180,392 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -411,161 +848,495 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:G11"/>
+  <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q11" sqref="Q11"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L26" sqref="L26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="1"/>
+    <col min="2" max="2" width="17.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B2" s="1" t="s">
+    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:7" s="13" customFormat="1" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="29">
+        <v>1</v>
+      </c>
+      <c r="B2" s="30" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B3" s="1" t="s">
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="32"/>
+    </row>
+    <row r="3" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="2">
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="17">
         <f>150</f>
         <v>150</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B4" s="1" t="s">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B4" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B5" s="1" t="s">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B5" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="3">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B7" s="1" t="s">
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="18">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B6" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="7">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="7">
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B8" s="33" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="18">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="34" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="1:7" s="13" customFormat="1" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="29">
+        <v>2</v>
+      </c>
+      <c r="B12" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="31"/>
+      <c r="D12" s="31"/>
+      <c r="E12" s="31"/>
+      <c r="F12" s="31"/>
+      <c r="G12" s="32"/>
+    </row>
+    <row r="13" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C13" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D13" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E13" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F13" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="G13" s="20" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B8" s="1" t="s">
+    <row r="14" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="1">
-        <f>D3</f>
+      <c r="C14" s="12">
+        <f>G3</f>
         <v>150</v>
       </c>
-      <c r="D8" s="1">
-        <f>IF($D$4="B",(2.5*LN($D$5/0.9834)+6.87)^2/345.6,IF($D$4="C",(2.5*LN($D$5/0.0984)+7.35)^2/478.4,(2.5*LN($D$5/0.0164)+7.65)^2/616.1))</f>
-        <v>1.0459270108559164</v>
-      </c>
-      <c r="E8" s="1">
+      <c r="D14" s="12">
+        <f>IF($G$4="B",(2.5*LN($G$5/0.9834)+6.87)^2/345.6,IF($G$4="C",(2.5*LN($G$5/0.0984)+7.35)^2/478.4,(2.5*LN($G$5/0.0164)+7.65)^2/616.1))</f>
+        <v>1.1428683287042622</v>
+      </c>
+      <c r="E14" s="12">
+        <f>$G$6</f>
         <v>0.85</v>
       </c>
-      <c r="F8" s="1">
-        <v>1.3</v>
-      </c>
-      <c r="G8" s="1">
-        <f>2.56*10^-6*C8^2*D8*E8*F8</f>
-        <v>6.6571162386957372E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B9" s="1" t="s">
+      <c r="F14" s="12">
+        <f>$G$7</f>
+        <v>1.6</v>
+      </c>
+      <c r="G14" s="19">
+        <f>2.56*10^-6*C14^2*D14*E14*F14</f>
+        <v>8.9527733397377088E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B15" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C15" s="6">
         <v>80</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D15" s="6">
         <v>1</v>
       </c>
-      <c r="E9" s="1">
+      <c r="E15" s="6">
         <v>1</v>
       </c>
-      <c r="F9" s="1">
-        <v>1.3</v>
-      </c>
-      <c r="G9" s="1">
-        <f t="shared" ref="G9:G11" si="0">2.56*10^-6*C9^2*D9*E9*F9</f>
-        <v>2.1299200000000001E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B10" s="1" t="s">
+      <c r="F15" s="6">
+        <f t="shared" ref="F15:F17" si="0">$G$7</f>
+        <v>1.6</v>
+      </c>
+      <c r="G15" s="7">
+        <f t="shared" ref="G15:G17" si="1">2.56*10^-6*C15^2*D15*E15*F15</f>
+        <v>2.6214399999999999E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B16" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C16" s="6">
         <v>70</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D16" s="6">
         <v>1</v>
       </c>
-      <c r="E10" s="1">
+      <c r="E16" s="6">
         <v>1</v>
       </c>
-      <c r="F10" s="1">
-        <v>1.3</v>
-      </c>
-      <c r="G10" s="1">
+      <c r="F16" s="6">
         <f t="shared" si="0"/>
-        <v>1.6307200000000001E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B11" s="1" t="s">
+        <v>1.6</v>
+      </c>
+      <c r="G16" s="7">
+        <f t="shared" si="1"/>
+        <v>2.0070400000000002E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="1">
-        <f>C8*0.75</f>
+      <c r="C17" s="9">
+        <f>C14*0.75</f>
         <v>112.5</v>
       </c>
-      <c r="D11" s="1">
-        <f t="shared" ref="D9:D11" si="1">IF($D$4="B",(2.5*LN($D$5/0.9834)+6.87)^2/345.6,IF($D$4="C",(2.5*LN($D$5/0.0984)+7.35)^2/478.4,(2.5*LN($D$5/0.0164)+7.65)^2/616.1))</f>
-        <v>1.0459270108559164</v>
-      </c>
-      <c r="E11" s="1">
+      <c r="D17" s="9">
+        <f>IF($G$4="B",(2.5*LN($G$5/0.9834)+6.87)^2/345.6,IF($G$4="C",(2.5*LN($G$5/0.0984)+7.35)^2/478.4,(2.5*LN($G$5/0.0164)+7.65)^2/616.1))</f>
+        <v>1.1428683287042622</v>
+      </c>
+      <c r="E17" s="9">
+        <f>$G$6</f>
         <v>0.85</v>
       </c>
-      <c r="F11" s="1">
-        <v>1.3</v>
-      </c>
-      <c r="G11" s="1">
+      <c r="F17" s="9">
         <f t="shared" si="0"/>
-        <v>3.7446278842663522E-2</v>
-      </c>
-    </row>
+        <v>1.6</v>
+      </c>
+      <c r="G17" s="16">
+        <f t="shared" si="1"/>
+        <v>5.0359350036024611E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="19" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="20" spans="1:7" s="13" customFormat="1" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="29">
+        <v>3</v>
+      </c>
+      <c r="B20" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20" s="31"/>
+      <c r="D20" s="31"/>
+      <c r="E20" s="31"/>
+      <c r="F20" s="31"/>
+      <c r="G20" s="32"/>
+    </row>
+    <row r="21" spans="1:7" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="D21" s="28"/>
+      <c r="E21" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="F21" s="28"/>
+      <c r="G21" s="28"/>
+    </row>
+    <row r="22" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="11">
+        <v>0</v>
+      </c>
+      <c r="C22" s="25">
+        <v>1</v>
+      </c>
+      <c r="D22" s="25"/>
+      <c r="E22" s="25">
+        <v>0</v>
+      </c>
+      <c r="F22" s="25"/>
+      <c r="G22" s="26"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B23" s="5">
+        <v>15</v>
+      </c>
+      <c r="C23" s="21">
+        <v>0.88</v>
+      </c>
+      <c r="D23" s="21"/>
+      <c r="E23" s="21">
+        <v>0.12</v>
+      </c>
+      <c r="F23" s="21"/>
+      <c r="G23" s="22"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B24" s="5">
+        <v>30</v>
+      </c>
+      <c r="C24" s="21">
+        <v>0.82</v>
+      </c>
+      <c r="D24" s="21"/>
+      <c r="E24" s="21">
+        <v>0.24</v>
+      </c>
+      <c r="F24" s="21"/>
+      <c r="G24" s="22"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B25" s="5">
+        <v>45</v>
+      </c>
+      <c r="C25" s="21">
+        <v>0.66</v>
+      </c>
+      <c r="D25" s="21"/>
+      <c r="E25" s="21">
+        <v>0.32</v>
+      </c>
+      <c r="F25" s="21"/>
+      <c r="G25" s="22"/>
+    </row>
+    <row r="26" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="8">
+        <v>60</v>
+      </c>
+      <c r="C26" s="23">
+        <v>0.34</v>
+      </c>
+      <c r="D26" s="23"/>
+      <c r="E26" s="23">
+        <v>0.38</v>
+      </c>
+      <c r="F26" s="23"/>
+      <c r="G26" s="24"/>
+    </row>
+    <row r="27" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="29" spans="1:7" s="13" customFormat="1" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="29">
+        <v>4</v>
+      </c>
+      <c r="B29" s="35" t="s">
+        <v>6</v>
+      </c>
+      <c r="C29" s="36"/>
+      <c r="D29" s="36"/>
+      <c r="E29" s="36"/>
+      <c r="F29" s="36"/>
+      <c r="G29" s="37"/>
+    </row>
+    <row r="30" spans="1:7" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="C30" s="28" t="s">
+        <v>24</v>
+      </c>
+      <c r="D30" s="28"/>
+      <c r="E30" s="28" t="s">
+        <v>25</v>
+      </c>
+      <c r="F30" s="28"/>
+      <c r="G30" s="28"/>
+    </row>
+    <row r="31" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="14">
+        <f>B22</f>
+        <v>0</v>
+      </c>
+      <c r="C31" s="3">
+        <f>$G$14*C22*$G$8*COS(RADIANS(B31))</f>
+        <v>0.80574960057639378</v>
+      </c>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3">
+        <f>$G$14*E22*$G$9*SIN(RADIANS(B31))</f>
+        <v>0</v>
+      </c>
+      <c r="F31" s="3"/>
+      <c r="G31" s="4"/>
+    </row>
+    <row r="32" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="5">
+        <f t="shared" ref="B32:B35" si="2">B23</f>
+        <v>15</v>
+      </c>
+      <c r="C32" s="3">
+        <f>$G$14*C23*$G$8*COS(RADIANS(B32))</f>
+        <v>0.68489902687257909</v>
+      </c>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3">
+        <f t="shared" ref="E32:E35" si="3">$G$14*E23*$G$9*SIN(RADIANS(B32))</f>
+        <v>2.5025201065550368E-2</v>
+      </c>
+      <c r="F32" s="3"/>
+      <c r="G32" s="4"/>
+    </row>
+    <row r="33" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="5">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+      <c r="C33" s="3">
+        <f t="shared" ref="C32:C35" si="4">$G$14*C24*$G$8*COS(RADIANS(B33))</f>
+        <v>0.57219569101442369</v>
+      </c>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3">
+        <f t="shared" si="3"/>
+        <v>9.6689952069167237E-2</v>
+      </c>
+      <c r="F33" s="3"/>
+      <c r="G33" s="4"/>
+    </row>
+    <row r="34" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="5">
+        <f t="shared" si="2"/>
+        <v>45</v>
+      </c>
+      <c r="C34" s="3">
+        <f t="shared" si="4"/>
+        <v>0.37603566429390739</v>
+      </c>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3">
+        <f t="shared" si="3"/>
+        <v>0.18232032208189444</v>
+      </c>
+      <c r="F34" s="3"/>
+      <c r="G34" s="4"/>
+    </row>
+    <row r="35" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B35" s="8">
+        <f t="shared" si="2"/>
+        <v>60</v>
+      </c>
+      <c r="C35" s="3">
+        <f t="shared" si="4"/>
+        <v>0.13697743209798699</v>
+      </c>
+      <c r="D35" s="3"/>
+      <c r="E35" s="3">
+        <f t="shared" si="3"/>
+        <v>0.26516385681156218</v>
+      </c>
+      <c r="F35" s="3"/>
+      <c r="G35" s="4"/>
+    </row>
+    <row r="36" spans="2:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
+  <mergeCells count="28">
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="E34:G34"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="E35:G35"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="E31:G31"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="E32:G32"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="E33:G33"/>
+    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="E24:G24"/>
+    <mergeCell ref="E25:G25"/>
+    <mergeCell ref="E26:G26"/>
+    <mergeCell ref="B29:G29"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="E30:G30"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="E22:G22"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="B12:G12"/>
+    <mergeCell ref="B20:G20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="E21:G21"/>
+    <mergeCell ref="C22:D22"/>
+  </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D4" xr:uid="{B4A8B5EF-A2F7-493D-80D0-9C0BBC970D7B}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G4" xr:uid="{B4A8B5EF-A2F7-493D-80D0-9C0BBC970D7B}">
       <formula1>"B, C, D"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
element local axes definition for elements have been created
</commit_message>
<xml_diff>
--- a/Spread sheet/Wind Load Generator.xlsx
+++ b/Spread sheet/Wind Load Generator.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wind_load_generator\Spread sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE8D0E5B-5971-4D85-B550-1469A1A923FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{990C3AA0-7D76-404C-B971-34DF15C8A25F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -466,9 +466,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -499,9 +496,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -515,34 +509,55 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -551,21 +566,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -850,8 +850,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L26" sqref="L26"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -863,449 +863,467 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:7" s="13" customFormat="1" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="29">
+    <row r="2" spans="1:7" s="12" customFormat="1" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="20">
         <v>1</v>
       </c>
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="32"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="37"/>
     </row>
     <row r="3" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="17">
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="15">
         <f>150</f>
         <v>150</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="7" t="s">
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="6" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="18">
-        <v>60</v>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="16">
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="7">
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="6">
         <v>0.85</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="7">
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="6">
         <v>1.6</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B8" s="33" t="s">
+      <c r="B8" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="18">
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="16">
         <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="34" t="s">
+      <c r="B9" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="10">
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="9">
         <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="12" spans="1:7" s="13" customFormat="1" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="29">
+    <row r="12" spans="1:7" s="12" customFormat="1" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="20">
         <v>2</v>
       </c>
-      <c r="B12" s="30" t="s">
+      <c r="B12" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="31"/>
-      <c r="D12" s="31"/>
-      <c r="E12" s="31"/>
-      <c r="F12" s="31"/>
-      <c r="G12" s="32"/>
+      <c r="C12" s="36"/>
+      <c r="D12" s="36"/>
+      <c r="E12" s="36"/>
+      <c r="F12" s="36"/>
+      <c r="G12" s="37"/>
     </row>
     <row r="13" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="20" t="s">
+      <c r="B13" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C13" s="20" t="s">
+      <c r="C13" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="D13" s="20" t="s">
+      <c r="D13" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="E13" s="20" t="s">
+      <c r="E13" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="F13" s="20" t="s">
+      <c r="F13" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="G13" s="20" t="s">
+      <c r="G13" s="18" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="11" t="s">
+      <c r="B14" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="12">
+      <c r="C14" s="11">
         <f>G3</f>
         <v>150</v>
       </c>
-      <c r="D14" s="12">
+      <c r="D14" s="11">
         <f>IF($G$4="B",(2.5*LN($G$5/0.9834)+6.87)^2/345.6,IF($G$4="C",(2.5*LN($G$5/0.0984)+7.35)^2/478.4,(2.5*LN($G$5/0.0164)+7.65)^2/616.1))</f>
-        <v>1.1428683287042622</v>
-      </c>
-      <c r="E14" s="12">
+        <v>1.0459270108559164</v>
+      </c>
+      <c r="E14" s="11">
         <f>$G$6</f>
         <v>0.85</v>
       </c>
-      <c r="F14" s="12">
+      <c r="F14" s="11">
         <f>$G$7</f>
         <v>1.6</v>
       </c>
-      <c r="G14" s="19">
+      <c r="G14" s="17">
         <f>2.56*10^-6*C14^2*D14*E14*F14</f>
-        <v>8.9527733397377088E-2</v>
+        <v>8.1933738322409078E-2</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="6">
+      <c r="C15" s="5">
         <v>80</v>
       </c>
-      <c r="D15" s="6">
+      <c r="D15" s="5">
         <v>1</v>
       </c>
-      <c r="E15" s="6">
+      <c r="E15" s="5">
         <v>1</v>
       </c>
-      <c r="F15" s="6">
+      <c r="F15" s="5">
         <f t="shared" ref="F15:F17" si="0">$G$7</f>
         <v>1.6</v>
       </c>
-      <c r="G15" s="7">
+      <c r="G15" s="6">
         <f t="shared" ref="G15:G17" si="1">2.56*10^-6*C15^2*D15*E15*F15</f>
         <v>2.6214399999999999E-2</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="6">
+      <c r="C16" s="5">
         <v>70</v>
       </c>
-      <c r="D16" s="6">
+      <c r="D16" s="5">
         <v>1</v>
       </c>
-      <c r="E16" s="6">
+      <c r="E16" s="5">
         <v>1</v>
       </c>
-      <c r="F16" s="6">
+      <c r="F16" s="5">
         <f t="shared" si="0"/>
         <v>1.6</v>
       </c>
-      <c r="G16" s="7">
+      <c r="G16" s="6">
         <f t="shared" si="1"/>
         <v>2.0070400000000002E-2</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="8" t="s">
+      <c r="B17" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C17" s="9">
+      <c r="C17" s="8">
         <f>C14*0.75</f>
         <v>112.5</v>
       </c>
-      <c r="D17" s="9">
+      <c r="D17" s="8">
         <f>IF($G$4="B",(2.5*LN($G$5/0.9834)+6.87)^2/345.6,IF($G$4="C",(2.5*LN($G$5/0.0984)+7.35)^2/478.4,(2.5*LN($G$5/0.0164)+7.65)^2/616.1))</f>
-        <v>1.1428683287042622</v>
-      </c>
-      <c r="E17" s="9">
+        <v>1.0459270108559164</v>
+      </c>
+      <c r="E17" s="8">
         <f>$G$6</f>
         <v>0.85</v>
       </c>
-      <c r="F17" s="9">
+      <c r="F17" s="8">
         <f t="shared" si="0"/>
         <v>1.6</v>
       </c>
-      <c r="G17" s="16">
+      <c r="G17" s="14">
         <f t="shared" si="1"/>
-        <v>5.0359350036024611E-2</v>
+        <v>4.6087727806355103E-2</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="19" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="20" spans="1:7" s="13" customFormat="1" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="29">
+    <row r="20" spans="1:7" s="12" customFormat="1" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="20">
         <v>3</v>
       </c>
-      <c r="B20" s="30" t="s">
+      <c r="B20" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="C20" s="31"/>
-      <c r="D20" s="31"/>
-      <c r="E20" s="31"/>
-      <c r="F20" s="31"/>
-      <c r="G20" s="32"/>
+      <c r="C20" s="36"/>
+      <c r="D20" s="36"/>
+      <c r="E20" s="36"/>
+      <c r="F20" s="36"/>
+      <c r="G20" s="37"/>
     </row>
     <row r="21" spans="1:7" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="27" t="s">
+      <c r="B21" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="C21" s="28" t="s">
+      <c r="C21" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="D21" s="28"/>
-      <c r="E21" s="28" t="s">
+      <c r="D21" s="32"/>
+      <c r="E21" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="F21" s="28"/>
-      <c r="G21" s="28"/>
+      <c r="F21" s="32"/>
+      <c r="G21" s="32"/>
     </row>
     <row r="22" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="11">
+      <c r="B22" s="10">
         <v>0</v>
       </c>
-      <c r="C22" s="25">
+      <c r="C22" s="33">
         <v>1</v>
       </c>
-      <c r="D22" s="25"/>
-      <c r="E22" s="25">
+      <c r="D22" s="33"/>
+      <c r="E22" s="33">
         <v>0</v>
       </c>
-      <c r="F22" s="25"/>
-      <c r="G22" s="26"/>
+      <c r="F22" s="33"/>
+      <c r="G22" s="34"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B23" s="5">
+      <c r="B23" s="4">
         <v>15</v>
       </c>
-      <c r="C23" s="21">
+      <c r="C23" s="25">
         <v>0.88</v>
       </c>
-      <c r="D23" s="21"/>
-      <c r="E23" s="21">
+      <c r="D23" s="25"/>
+      <c r="E23" s="25">
         <v>0.12</v>
       </c>
-      <c r="F23" s="21"/>
-      <c r="G23" s="22"/>
+      <c r="F23" s="25"/>
+      <c r="G23" s="26"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B24" s="5">
+      <c r="B24" s="4">
         <v>30</v>
       </c>
-      <c r="C24" s="21">
+      <c r="C24" s="25">
         <v>0.82</v>
       </c>
-      <c r="D24" s="21"/>
-      <c r="E24" s="21">
+      <c r="D24" s="25"/>
+      <c r="E24" s="25">
         <v>0.24</v>
       </c>
-      <c r="F24" s="21"/>
-      <c r="G24" s="22"/>
+      <c r="F24" s="25"/>
+      <c r="G24" s="26"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B25" s="5">
+      <c r="B25" s="4">
         <v>45</v>
       </c>
-      <c r="C25" s="21">
+      <c r="C25" s="25">
         <v>0.66</v>
       </c>
-      <c r="D25" s="21"/>
-      <c r="E25" s="21">
+      <c r="D25" s="25"/>
+      <c r="E25" s="25">
         <v>0.32</v>
       </c>
-      <c r="F25" s="21"/>
-      <c r="G25" s="22"/>
+      <c r="F25" s="25"/>
+      <c r="G25" s="26"/>
     </row>
     <row r="26" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="8">
+      <c r="B26" s="7">
         <v>60</v>
       </c>
-      <c r="C26" s="23">
+      <c r="C26" s="27">
         <v>0.34</v>
       </c>
-      <c r="D26" s="23"/>
-      <c r="E26" s="23">
+      <c r="D26" s="27"/>
+      <c r="E26" s="27">
         <v>0.38</v>
       </c>
-      <c r="F26" s="23"/>
-      <c r="G26" s="24"/>
+      <c r="F26" s="27"/>
+      <c r="G26" s="28"/>
     </row>
     <row r="27" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="28" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="29" spans="1:7" s="13" customFormat="1" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="29">
+    <row r="29" spans="1:7" s="12" customFormat="1" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="20">
         <v>4</v>
       </c>
-      <c r="B29" s="35" t="s">
+      <c r="B29" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="C29" s="36"/>
-      <c r="D29" s="36"/>
-      <c r="E29" s="36"/>
-      <c r="F29" s="36"/>
-      <c r="G29" s="37"/>
+      <c r="C29" s="30"/>
+      <c r="D29" s="30"/>
+      <c r="E29" s="30"/>
+      <c r="F29" s="30"/>
+      <c r="G29" s="31"/>
     </row>
     <row r="30" spans="1:7" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="27" t="s">
+      <c r="B30" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="C30" s="28" t="s">
+      <c r="C30" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="D30" s="28"/>
-      <c r="E30" s="28" t="s">
+      <c r="D30" s="32"/>
+      <c r="E30" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="F30" s="28"/>
-      <c r="G30" s="28"/>
+      <c r="F30" s="32"/>
+      <c r="G30" s="32"/>
     </row>
     <row r="31" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="14">
+      <c r="B31" s="13">
         <f>B22</f>
         <v>0</v>
       </c>
-      <c r="C31" s="3">
+      <c r="C31" s="23">
         <f>$G$14*C22*$G$8*COS(RADIANS(B31))</f>
-        <v>0.80574960057639378</v>
-      </c>
-      <c r="D31" s="3"/>
-      <c r="E31" s="3">
+        <v>0.73740364490168164</v>
+      </c>
+      <c r="D31" s="23"/>
+      <c r="E31" s="23">
         <f>$G$14*E22*$G$9*SIN(RADIANS(B31))</f>
         <v>0</v>
       </c>
-      <c r="F31" s="3"/>
-      <c r="G31" s="4"/>
+      <c r="F31" s="23"/>
+      <c r="G31" s="24"/>
     </row>
     <row r="32" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="5">
+      <c r="B32" s="4">
         <f t="shared" ref="B32:B35" si="2">B23</f>
         <v>15</v>
       </c>
-      <c r="C32" s="3">
+      <c r="C32" s="23">
         <f>$G$14*C23*$G$8*COS(RADIANS(B32))</f>
-        <v>0.68489902687257909</v>
-      </c>
-      <c r="D32" s="3"/>
-      <c r="E32" s="3">
+        <v>0.62680395800900024</v>
+      </c>
+      <c r="D32" s="23"/>
+      <c r="E32" s="23">
         <f t="shared" ref="E32:E35" si="3">$G$14*E23*$G$9*SIN(RADIANS(B32))</f>
-        <v>2.5025201065550368E-2</v>
-      </c>
-      <c r="F32" s="3"/>
-      <c r="G32" s="4"/>
+        <v>2.2902492867428587E-2</v>
+      </c>
+      <c r="F32" s="23"/>
+      <c r="G32" s="24"/>
     </row>
     <row r="33" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="5">
+      <c r="B33" s="4">
         <f t="shared" si="2"/>
         <v>30</v>
       </c>
-      <c r="C33" s="3">
-        <f t="shared" ref="C32:C35" si="4">$G$14*C24*$G$8*COS(RADIANS(B33))</f>
-        <v>0.57219569101442369</v>
-      </c>
-      <c r="D33" s="3"/>
-      <c r="E33" s="3">
+      <c r="C33" s="23">
+        <f t="shared" ref="C33:C35" si="4">$G$14*C24*$G$8*COS(RADIANS(B33))</f>
+        <v>0.52366043724903855</v>
+      </c>
+      <c r="D33" s="23"/>
+      <c r="E33" s="23">
         <f t="shared" si="3"/>
-        <v>9.6689952069167237E-2</v>
-      </c>
-      <c r="F33" s="3"/>
-      <c r="G33" s="4"/>
+        <v>8.8488437388201793E-2</v>
+      </c>
+      <c r="F33" s="23"/>
+      <c r="G33" s="24"/>
     </row>
     <row r="34" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="5">
+      <c r="B34" s="4">
         <f t="shared" si="2"/>
         <v>45</v>
       </c>
-      <c r="C34" s="3">
+      <c r="C34" s="23">
         <f t="shared" si="4"/>
-        <v>0.37603566429390739</v>
-      </c>
-      <c r="D34" s="3"/>
-      <c r="E34" s="3">
+        <v>0.34413925773589299</v>
+      </c>
+      <c r="D34" s="23"/>
+      <c r="E34" s="23">
         <f t="shared" si="3"/>
-        <v>0.18232032208189444</v>
-      </c>
-      <c r="F34" s="3"/>
-      <c r="G34" s="4"/>
+        <v>0.16685539769012991</v>
+      </c>
+      <c r="F34" s="23"/>
+      <c r="G34" s="24"/>
     </row>
     <row r="35" spans="2:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="8">
+      <c r="B35" s="7">
         <f t="shared" si="2"/>
         <v>60</v>
       </c>
-      <c r="C35" s="3">
+      <c r="C35" s="23">
         <f t="shared" si="4"/>
-        <v>0.13697743209798699</v>
-      </c>
-      <c r="D35" s="3"/>
-      <c r="E35" s="3">
+        <v>0.12535861963328593</v>
+      </c>
+      <c r="D35" s="23"/>
+      <c r="E35" s="23">
         <f t="shared" si="3"/>
-        <v>0.26516385681156218</v>
-      </c>
-      <c r="F35" s="3"/>
-      <c r="G35" s="4"/>
+        <v>0.24267190994467636</v>
+      </c>
+      <c r="F35" s="23"/>
+      <c r="G35" s="24"/>
     </row>
     <row r="36" spans="2:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="E22:G22"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="B12:G12"/>
+    <mergeCell ref="B20:G20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="E21:G21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="E30:G30"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="E24:G24"/>
+    <mergeCell ref="E25:G25"/>
+    <mergeCell ref="E26:G26"/>
+    <mergeCell ref="B29:G29"/>
     <mergeCell ref="C34:D34"/>
     <mergeCell ref="E34:G34"/>
     <mergeCell ref="C35:D35"/>
@@ -1316,24 +1334,6 @@
     <mergeCell ref="E32:G32"/>
     <mergeCell ref="C33:D33"/>
     <mergeCell ref="E33:G33"/>
-    <mergeCell ref="E23:G23"/>
-    <mergeCell ref="E24:G24"/>
-    <mergeCell ref="E25:G25"/>
-    <mergeCell ref="E26:G26"/>
-    <mergeCell ref="B29:G29"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="E30:G30"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="E22:G22"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="B12:G12"/>
-    <mergeCell ref="B20:G20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="E21:G21"/>
-    <mergeCell ref="C22:D22"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G4" xr:uid="{B4A8B5EF-A2F7-493D-80D0-9C0BBC970D7B}">

</xml_diff>